<commit_message>
Added sm for temp
</commit_message>
<xml_diff>
--- a/questions/ServerCommandTableA8.xlsx
+++ b/questions/ServerCommandTableA8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CU-B\IOT\W3\New folder\ecen5823-assignment8-anuh7\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F624094-BE01-4D73-849E-50E2F8390BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F00446-5174-4382-BFED-B58DFFC458A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="-14430" windowWidth="16230" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -213,10 +213,6 @@
 Gattdb_button_state: same-led1. </t>
   </si>
   <si>
-    <t>?? When is indication_inflight cleared?
-sl_bt_evt_gatt_server_indication_timeout_id???</t>
-  </si>
-  <si>
     <t>DISPLAY_ROW_9, Button pressed/released</t>
   </si>
   <si>
@@ -227,7 +223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -671,15 +667,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -732,6 +719,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,23 +818,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1126901</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>73589</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1175674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1781578</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>128186</xdr:rowOff>
+      <xdr:colOff>1921100</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>40197</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22DA015E-2575-A821-1C8E-37E92C6AD8E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C88D2AD3-7B63-939F-4278-A656B50B0308}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -854,8 +850,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4893971" y="10119110"/>
-          <a:ext cx="7480479" cy="4175836"/>
+          <a:off x="5977944" y="14022350"/>
+          <a:ext cx="6922395" cy="4230720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1947,11 +1943,11 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" style="1" customWidth="1"/>
@@ -1964,18 +1960,18 @@
     <col min="9" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="14.55" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="2" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61"/>
+    </row>
+    <row r="2" spans="1:7" ht="12" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -1984,7 +1980,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="119.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="119.55" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -2000,7 +1996,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="12" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -2021,7 +2017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="34.799999999999997" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
@@ -2032,7 +2028,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="26.4" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
         <v>9</v>
@@ -2047,7 +2043,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="13.5" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="13"/>
@@ -2060,10 +2056,10 @@
       </c>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="28.2" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="39" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="30"/>
@@ -2073,7 +2069,7 @@
       <c r="F8" s="32"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="13.5" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
@@ -2084,36 +2080,36 @@
       <c r="F9" s="27"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" ht="26.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="26.7" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="30"/>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="52" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7" ht="26.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26.7" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="30"/>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="52" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="26.4" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="40" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="30"/>
@@ -2123,7 +2119,7 @@
       <c r="F12" s="27"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="13.5" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="15"/>
@@ -2131,7 +2127,7 @@
       <c r="F13" s="26"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="28.8" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="16" t="s">
         <v>11</v>
@@ -2148,7 +2144,7 @@
       </c>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="13.2" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
@@ -2159,7 +2155,7 @@
       <c r="F15" s="26"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="13.2" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
@@ -2168,7 +2164,7 @@
       <c r="F16" s="26"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="28.2" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="16" t="s">
         <v>12</v>
@@ -2179,7 +2175,7 @@
       <c r="D17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="53" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="27" t="s">
@@ -2187,7 +2183,7 @@
       </c>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="37.799999999999997" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15" t="s">
@@ -2200,7 +2196,7 @@
       <c r="F18" s="26"/>
       <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="13.5" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
@@ -2208,7 +2204,7 @@
       <c r="F19" s="37"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="13.5" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="16" t="s">
         <v>13</v>
@@ -2218,22 +2214,22 @@
       <c r="E20" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="46"/>
-    </row>
-    <row r="21" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="43"/>
+    </row>
+    <row r="21" spans="1:7" ht="55.2" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
       <c r="D21" s="24"/>
-      <c r="E21" s="56" t="s">
+      <c r="E21" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="37.200000000000003" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
@@ -2242,45 +2238,45 @@
       <c r="F22" s="26"/>
       <c r="G22" s="34"/>
     </row>
-    <row r="23" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="78.75" customHeight="1">
       <c r="A23" s="4"/>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="57" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="15"/>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="54" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="19"/>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="13.5" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="58"/>
+      <c r="E24" s="55"/>
       <c r="F24" s="18"/>
       <c r="G24" s="28"/>
     </row>
-    <row r="25" spans="1:7" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="61.2" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="21"/>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="56" t="s">
         <v>33</v>
       </c>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="76.8" customHeight="1">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>32</v>
@@ -2290,44 +2286,44 @@
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="47" t="s">
+      <c r="F26" s="44" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="33.6" customHeight="1">
       <c r="A27" s="4"/>
       <c r="B27" s="16"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="50"/>
-    </row>
-    <row r="28" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="49"/>
+      <c r="G27" s="47"/>
+    </row>
+    <row r="28" spans="1:7" ht="13.5" customHeight="1">
       <c r="A28" s="4"/>
-      <c r="B28" s="54"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
-      <c r="E28" s="48"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="36"/>
       <c r="G28" s="26"/>
     </row>
-    <row r="29" spans="1:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="53"/>
+    <row r="29" spans="1:7" ht="52.8" customHeight="1">
+      <c r="A29" s="50"/>
       <c r="B29" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="24"/>
-      <c r="E29" s="49"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="35"/>
       <c r="G29" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="62.4" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
@@ -2338,11 +2334,11 @@
         <v>49</v>
       </c>
       <c r="D30" s="15"/>
-      <c r="E30" s="61"/>
+      <c r="E30" s="58"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="51"/>
-    </row>
-    <row r="31" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="48"/>
+    </row>
+    <row r="31" spans="1:7" ht="13.5" customHeight="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>36</v>
@@ -2350,22 +2346,20 @@
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="15"/>
     </row>
-    <row r="32" spans="1:7" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="111.6" customHeight="1">
       <c r="A32" s="4"/>
       <c r="B32" s="16"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="F32" s="19"/>
-      <c r="G32" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="1:7" ht="13.5" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
@@ -2374,7 +2368,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="13.5" customHeight="1">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>

</xml_diff>